<commit_message>
updated Excel template. result_type removed
</commit_message>
<xml_diff>
--- a/public/MagIC/help/Template3.0ForMagICUpload.xlsx
+++ b/public/MagIC/help/Template3.0ForMagICUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njarboe/Dropbox/MagIC/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njarboe/git/earthref/MagIC/public/MagIC/help/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C238F40-9955-BD45-B1B0-EE9D8F422C43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6A7B6A-6D6B-9C4F-A9FB-7D0502EA0191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21500" yWindow="8140" windowWidth="28800" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="4340" windowWidth="40660" windowHeight="17560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
   <si>
     <t>location</t>
   </si>
@@ -286,9 +286,6 @@
     <t>integer that increases for each measurement</t>
   </si>
   <si>
-    <t>u=unknown or s=a standard (calibration) measurement</t>
-  </si>
-  <si>
     <t>g=good, b=bad</t>
   </si>
   <si>
@@ -317,6 +314,15 @@
   </si>
   <si>
     <t>external_database_ids</t>
+  </si>
+  <si>
+    <t>u= unknown or s=standard (calibration) measurement</t>
+  </si>
+  <si>
+    <t>dir_tilt_correction</t>
+  </si>
+  <si>
+    <t>Use 0 for geographic and 100 for straigraphic correction. See online data model (earthref.org/MagIC/data-models/3.0) for more options</t>
   </si>
 </sst>
 </file>
@@ -745,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -765,16 +771,16 @@
         <v>51</v>
       </c>
       <c r="O1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" t="s">
         <v>88</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>90</v>
-      </c>
-      <c r="R1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -858,10 +864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,20 +875,24 @@
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="18.1640625" customWidth="1"/>
-    <col min="20" max="20" width="12.5" customWidth="1"/>
-    <col min="21" max="21" width="6.1640625" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" customWidth="1"/>
-    <col min="26" max="26" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" customWidth="1"/>
+    <col min="19" max="19" width="13" customWidth="1"/>
+    <col min="20" max="20" width="18.1640625" customWidth="1"/>
+    <col min="21" max="21" width="12.5" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -935,30 +945,33 @@
         <v>34</v>
       </c>
       <c r="R2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1099,14 +1112,14 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" customWidth="1"/>
@@ -1164,22 +1177,22 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
         <v>82</v>
       </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" t="s">
         <v>84</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>85</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>86</v>
-      </c>
-      <c r="M2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1193,19 +1206,19 @@
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>30</v>
@@ -1258,7 +1271,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{D9599BEB-D39E-E94A-A11B-EECB49B8CECA}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{D9599BEB-D39E-E94A-A11B-EECB49B8CECA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1329,7 +1342,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
         <v>47</v>
@@ -1373,7 +1386,7 @@
         <v>17</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>